<commit_message>
modify the db file
</commit_message>
<xml_diff>
--- a/guide/db.xlsx
+++ b/guide/db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pch88\Desktop\gourminati\gourminati\guide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pch88\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DD53F0-B103-4693-96BC-2A6D50457C40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00DB35A-D83D-443A-9001-A7DD49994029}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="2445" windowWidth="16185" windowHeight="10935" xr2:uid="{D1263C40-323A-4C3D-8A6A-64A59C4E42F9}"/>
+    <workbookView xWindow="19410" yWindow="165" windowWidth="13380" windowHeight="13380" xr2:uid="{D1263C40-323A-4C3D-8A6A-64A59C4E42F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="121">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -212,16 +212,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>서울 중구 삼일대로12길 16</t>
-  </si>
-  <si>
     <t>순남시래기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>서울 서초구 강남대로39길 15-10</t>
-  </si>
-  <si>
     <t>유래회관</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -241,9 +235,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>서울 중구 서소문로 134-7</t>
-  </si>
-  <si>
     <t>대구형제막창</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -407,13 +398,6 @@
     <t>인천 남동구 남동대로 467</t>
   </si>
   <si>
-    <t>로쿠베스시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제주특별자치도 서귀포시 중앙로 81</t>
-  </si>
-  <si>
     <t>parking</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -440,13 +424,526 @@
   <si>
     <t>$$$</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>농민백암순대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강남구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선릉로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>86</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>길</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 40-4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알앤지타운</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>육류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 강남구 선릉로86길 6-5 (우)06198</t>
+  </si>
+  <si>
+    <t>room</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삼일대로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>길</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 16</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서초구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강남대로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>39</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>길</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 15-10</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서소문로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 134-7</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>남대문로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>길</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 16</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화포식당</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈그리아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배꼽집</t>
+  </si>
+  <si>
+    <t>시래마루</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경기 광주시 곤지암읍 경충대로 661 1층</t>
+  </si>
+  <si>
+    <t>$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$$$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소고기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 강남구 강남대로128길 22</t>
+  </si>
+  <si>
+    <t>우성토종한우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경기 의왕시 왕송못서길 106</t>
+  </si>
+  <si>
+    <t>가시아방국수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제주도도야지생삼겹살</t>
+  </si>
+  <si>
+    <t>육류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경기 수원시 장안구 서부로2105번길 16-23</t>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제주특별자치도 서귀포시 성산읍 섭지코지로 10 1층</t>
+  </si>
+  <si>
+    <t>국수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시골밥상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한정식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강원 정선군 사북읍 사북중앙로 67</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +994,20 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -520,7 +1031,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -534,6 +1045,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -850,20 +1364,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058F4786-AE65-4888-AE95-4CF079DCAE1F}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -877,13 +1391,16 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -897,13 +1414,16 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -917,13 +1437,16 @@
         <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -937,13 +1460,16 @@
         <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -957,13 +1483,16 @@
         <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -977,13 +1506,16 @@
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -997,13 +1529,16 @@
         <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1017,13 +1552,16 @@
         <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1037,13 +1575,16 @@
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1057,13 +1598,16 @@
         <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1077,13 +1621,16 @@
         <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1097,13 +1644,16 @@
         <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1117,13 +1667,16 @@
         <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1137,13 +1690,16 @@
         <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1157,13 +1713,16 @@
         <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="G15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1173,274 +1732,500 @@
       <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
+      <c r="D16" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>47</v>
+      <c r="D17" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="G18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="G21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="E23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F29" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="G29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" t="s">
+        <v>87</v>
+      </c>
+      <c r="G31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" t="s">
+        <v>103</v>
+      </c>
+      <c r="G34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F35" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" t="s">
+        <v>112</v>
+      </c>
+      <c r="F36" t="s">
+        <v>113</v>
+      </c>
+      <c r="G36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" t="s">
+        <v>116</v>
+      </c>
+      <c r="F37" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>